<commit_message>
added in some UI Validation
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikegajda/Documents/Projects/411/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="15360" windowHeight="20020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>form field validation</t>
   </si>
@@ -73,19 +81,97 @@
   </si>
   <si>
     <t>adele</t>
+  </si>
+  <si>
+    <t>UI Validation</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>UI Element</t>
+  </si>
+  <si>
+    <t>Expected Function</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Pass/fail</t>
+  </si>
+  <si>
+    <t>Sign in with Facebook</t>
+  </si>
+  <si>
+    <t>Sign in with Twitter</t>
+  </si>
+  <si>
+    <t>Sign in with Google</t>
+  </si>
+  <si>
+    <t>Sign in with Github</t>
+  </si>
+  <si>
+    <t>Sign in with Linkedin</t>
+  </si>
+  <si>
+    <t>Sign in with Instagram</t>
+  </si>
+  <si>
+    <t>ui.1</t>
+  </si>
+  <si>
+    <t>ui.2</t>
+  </si>
+  <si>
+    <t>ui.3</t>
+  </si>
+  <si>
+    <t>ui.4</t>
+  </si>
+  <si>
+    <t>ui.5</t>
+  </si>
+  <si>
+    <t>ui.6</t>
+  </si>
+  <si>
+    <t>Successfully login with Facebook</t>
+  </si>
+  <si>
+    <t>Successfully login with Twitter</t>
+  </si>
+  <si>
+    <t>Successfully login with Google</t>
+  </si>
+  <si>
+    <t>Successfully login with Github</t>
+  </si>
+  <si>
+    <t>Successfully login with Linkedin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully login with Instagram </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,14 +194,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -441,24 +533,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -475,7 +568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -492,7 +585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -509,7 +602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -526,7 +619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -540,7 +633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -554,7 +647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -571,7 +664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -588,12 +681,134 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more ui tests
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>form field validation</t>
   </si>
@@ -153,6 +153,75 @@
   </si>
   <si>
     <t xml:space="preserve">Successfully login with Instagram </t>
+  </si>
+  <si>
+    <t>index (upon login)</t>
+  </si>
+  <si>
+    <t>Find party (nothing in Party ID field)</t>
+  </si>
+  <si>
+    <t>Flash error saying "party id must be exactly 24 characters long."</t>
+  </si>
+  <si>
+    <t>ui.7</t>
+  </si>
+  <si>
+    <t>Find party (Party ID in field)</t>
+  </si>
+  <si>
+    <t>redirect to proper party</t>
+  </si>
+  <si>
+    <t>ui.8</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>create new party, and redirect</t>
+  </si>
+  <si>
+    <t>ui.9</t>
+  </si>
+  <si>
+    <t>party/:partyid</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>No function expected, because the angular frontend will automatically load what is in the Query field</t>
+  </si>
+  <si>
+    <t>Vote up</t>
+  </si>
+  <si>
+    <t>ui.10</t>
+  </si>
+  <si>
+    <t>ui.11</t>
+  </si>
+  <si>
+    <t>ui.12</t>
+  </si>
+  <si>
+    <t>Vote down</t>
+  </si>
+  <si>
+    <t>Number of votes for song increases</t>
+  </si>
+  <si>
+    <t>Number of votes for song decreases</t>
+  </si>
+  <si>
+    <t>+' (add song to queue)</t>
+  </si>
+  <si>
+    <t>Song shows up in queue</t>
+  </si>
+  <si>
+    <t>ui.13</t>
   </si>
 </sst>
 </file>
@@ -194,9 +263,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,15 +606,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
@@ -808,6 +882,125 @@
         <v>10</v>
       </c>
     </row>
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added data validation attempt/ prototype to testing.xlsx.
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11080" yWindow="0" windowWidth="25360" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="11076" yWindow="0" windowWidth="20376" windowHeight="12816" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Testing" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,12 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="201">
   <si>
     <t>index</t>
   </si>
@@ -300,9 +297,6 @@
     <t>"</t>
   </si>
   <si>
-    <t>question mark, quotation marks and empty string cause it to fail</t>
-  </si>
-  <si>
     <t>form.3, form.4, and form.5</t>
   </si>
   <si>
@@ -496,13 +490,145 @@
   </si>
   <si>
     <t>form.20</t>
+  </si>
+  <si>
+    <t>special characters and empty string or any string containing them, cause it to fail</t>
+  </si>
+  <si>
+    <t>PartySchema</t>
+  </si>
+  <si>
+    <t>user_ids</t>
+  </si>
+  <si>
+    <t>Array of Stings</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>data.1</t>
+  </si>
+  <si>
+    <t>Index.Create</t>
+  </si>
+  <si>
+    <t>(spotify access token)</t>
+  </si>
+  <si>
+    <t>host_id</t>
+  </si>
+  <si>
+    <t>5722d43843ff22bc1be4bdbe</t>
+  </si>
+  <si>
+    <t>data.2</t>
+  </si>
+  <si>
+    <t>song_ids</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>data.3</t>
+  </si>
+  <si>
+    <t>Array of Objects</t>
+  </si>
+  <si>
+    <t>qr_code</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>(qr-api url + ip adress)</t>
+  </si>
+  <si>
+    <t>data.4</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>paty.add song to queue</t>
+  </si>
+  <si>
+    <t>(song object)</t>
+  </si>
+  <si>
+    <t>data.5</t>
+  </si>
+  <si>
+    <t>song_ids.votes</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>data.6</t>
+  </si>
+  <si>
+    <t>party.partyid</t>
+  </si>
+  <si>
+    <t>data.7</t>
+  </si>
+  <si>
+    <t>party.Vote</t>
+  </si>
+  <si>
+    <t>(test value not applicable)</t>
+  </si>
+  <si>
+    <t>SearchResultSchema</t>
+  </si>
+  <si>
+    <t>party.search</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>50kpGaPAhYJ3sGmk6vplg0</t>
+  </si>
+  <si>
+    <t>data.8</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>"Love Yourself"</t>
+  </si>
+  <si>
+    <t>data.9</t>
+  </si>
+  <si>
+    <t>artists</t>
+  </si>
+  <si>
+    <t>Justin Bieber</t>
+  </si>
+  <si>
+    <t>data.10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -543,6 +669,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -574,7 +720,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -594,7 +740,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -937,23 +1092,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:I63"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.296875" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="13.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.69921875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -965,8 +1122,9 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -985,8 +1143,9 @@
       <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -999,14 +1158,14 @@
       <c r="D3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1083,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1100,7 +1259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1120,7 +1279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1131,7 +1290,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
@@ -1140,7 +1299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1151,7 +1310,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>91</v>
@@ -1160,55 +1319,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>6</v>
@@ -1217,18 +1376,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="1">
         <v>256324234</v>
@@ -1237,96 +1396,96 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15">
+    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="F18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E19"/>
       <c r="F19" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>91</v>
@@ -1335,18 +1494,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15">
+    <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -1355,30 +1514,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1388,12 +1547,13 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="20">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="A26" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B26" s="6"/>
@@ -1404,8 +1564,9 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>77</v>
       </c>
@@ -1424,718 +1585,1077 @@
       <c r="F27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" ht="20">
-      <c r="A33" s="6" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="A44" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="2" t="s">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="1" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="1" t="s">
+      <c r="E46" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="1" t="s">
+      <c r="E47" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="1" t="s">
+      <c r="E48" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="1" t="s">
+      <c r="E49" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1" t="s">
+      <c r="E50" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="28">
-      <c r="A41" s="1" t="s">
+      <c r="E51" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1" t="s">
+      <c r="E52" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="1" t="s">
+      <c r="E53" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="42">
-      <c r="A44" s="1" t="s">
+      <c r="E54" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="1" t="s">
+      <c r="E55" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="1" t="s">
+      <c r="E56" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="1" t="s">
+      <c r="E57" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="1" t="s">
+      <c r="E58" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="D59" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="28">
-      <c r="A49" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-    </row>
-    <row r="50" spans="1:9" ht="42">
-      <c r="A50" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>136</v>
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E61" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
-    </row>
-    <row r="63" spans="1:9" ht="20">
-      <c r="A63" s="6" t="s">
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="74" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="A74" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="2" t="s">
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="28">
-      <c r="A65" s="1" t="s">
+    <row r="76" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" s="4">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E77" s="4">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E78" s="4">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" s="4">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C80" s="1">
+        <v>2</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E80" s="4">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C65" s="1">
+      <c r="B81" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="1">
         <v>1</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E65" s="4">
-        <v>42484</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" s="1">
-        <v>1</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E66" s="4">
-        <v>42484</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="28">
-      <c r="A67" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C67" s="1">
-        <v>1</v>
-      </c>
-      <c r="D67" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E67" s="4">
-        <v>42484</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="28">
-      <c r="A68" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68" s="4">
-        <v>42484</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="28">
-      <c r="A69" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="1">
-        <v>2</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E69" s="4">
-        <v>42484</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E70" s="4">
+      <c r="E81" s="4">
         <v>42484</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A63:I63"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A44:J44"/>
+    <mergeCell ref="A74:J74"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Finished up more of the data validation prototype. Still unsure about it.
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="214">
   <si>
     <t>index</t>
   </si>
@@ -543,9 +543,6 @@
     <t>w</t>
   </si>
   <si>
-    <t>(qr-api url + ip adress)</t>
-  </si>
-  <si>
     <t>data.4</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t>party.Vote</t>
   </si>
   <si>
-    <t>(test value not applicable)</t>
-  </si>
-  <si>
     <t>SearchResultSchema</t>
   </si>
   <si>
@@ -609,9 +603,6 @@
     <t>users</t>
   </si>
   <si>
-    <t>"Love Yourself"</t>
-  </si>
-  <si>
     <t>data.9</t>
   </si>
   <si>
@@ -622,6 +613,54 @@
   </si>
   <si>
     <t>data.10</t>
+  </si>
+  <si>
+    <t>(qr-api url + party_id)</t>
+  </si>
+  <si>
+    <t>duration_ms</t>
+  </si>
+  <si>
+    <t>data.11</t>
+  </si>
+  <si>
+    <t>search href</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String </t>
+  </si>
+  <si>
+    <t>data.12</t>
+  </si>
+  <si>
+    <t>song href</t>
+  </si>
+  <si>
+    <t>data.13</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>account.signup</t>
+  </si>
+  <si>
+    <t>String, unique</t>
+  </si>
+  <si>
+    <t>Love Yourself</t>
+  </si>
+  <si>
+    <t>whatever@bu.edu</t>
+  </si>
+  <si>
+    <t>data.14</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.15 </t>
   </si>
 </sst>
 </file>
@@ -713,14 +752,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -737,14 +777,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -752,12 +786,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1092,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1111,18 +1155,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1158,7 +1202,7 @@
       <c r="D3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1553,18 +1597,18 @@
       <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -1585,7 +1629,7 @@
       <c r="F27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="7" t="s">
         <v>71</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -1596,432 +1640,500 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>159</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="6" t="s">
         <v>164</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>161</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="H30" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="H30" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C31" s="10" t="s">
+      <c r="E34" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D35" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E31" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="F31" s="10" t="s">
+      <c r="E41" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="D42" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="E42" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
+      <c r="G42" s="8">
+        <v>1234</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-    </row>
-    <row r="44" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A44" s="6" t="s">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+    </row>
+    <row r="46" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="A46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -2029,13 +2141,13 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>4</v>
@@ -2046,13 +2158,13 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>4</v>
@@ -2063,13 +2175,13 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>4</v>
@@ -2080,30 +2192,30 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>4</v>
@@ -2111,50 +2223,50 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>4</v>
@@ -2162,33 +2274,33 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>4</v>
@@ -2198,14 +2310,14 @@
       <c r="A58" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>54</v>
+      <c r="B58" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>4</v>
@@ -2213,77 +2325,67 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-    </row>
-    <row r="61" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E61" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>4</v>
@@ -2294,18 +2396,18 @@
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>4</v>
@@ -2317,17 +2419,17 @@
       <c r="J63" s="5"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>4</v>
@@ -2343,13 +2445,13 @@
         <v>100</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>4</v>
@@ -2365,13 +2467,13 @@
         <v>100</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>4</v>
@@ -2387,13 +2489,13 @@
         <v>100</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>4</v>
@@ -2409,13 +2511,13 @@
         <v>100</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>4</v>
@@ -2431,13 +2533,13 @@
         <v>100</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>4</v>
@@ -2450,18 +2552,18 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E70" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F70" s="5"/>
@@ -2472,18 +2574,18 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E71" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F71" s="5"/>
@@ -2497,13 +2599,13 @@
         <v>102</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>4</v>
@@ -2514,100 +2616,110 @@
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="74" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A74" s="6" t="s">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="76" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="A76" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E77" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C76" s="1">
-        <v>1</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E76" s="4">
-        <v>42484</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C77" s="1">
-        <v>1</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E77" s="4">
-        <v>42484</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C78" s="1">
         <v>1</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E78" s="4">
         <v>42484</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="C79" s="1">
         <v>1</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="E79" s="4">
         <v>42484</v>
@@ -2615,27 +2727,27 @@
     </row>
     <row r="80" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C80" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E80" s="4">
         <v>42484</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C81" s="1">
         <v>1</v>
@@ -2644,6 +2756,40 @@
         <v>86</v>
       </c>
       <c r="E81" s="4">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" s="1">
+        <v>2</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E82" s="4">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C83" s="1">
+        <v>1</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83" s="4">
         <v>42484</v>
       </c>
     </row>
@@ -2651,11 +2797,14 @@
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A26:J26"/>
-    <mergeCell ref="A44:J44"/>
-    <mergeCell ref="A74:J74"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="A76:J76"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G41" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>